<commit_message>
Update other test sheets
</commit_message>
<xml_diff>
--- a/test_data/test_3.xlsx
+++ b/test_data/test_3.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daveih/Documents/python/usdm_data/test_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52C9BCDA-D689-354B-A37A-AB7D9509C152}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91E79F30-362F-6042-A682-DA5BB692BFD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="520" windowWidth="33600" windowHeight="19480" activeTab="1" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
+    <workbookView xWindow="20340" yWindow="6800" windowWidth="33600" windowHeight="19480" firstSheet="4" activeTab="5" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
   </bookViews>
   <sheets>
     <sheet name="study" sheetId="2" r:id="rId1"/>
@@ -18,13 +18,15 @@
     <sheet name="mainTimeline" sheetId="1" r:id="rId3"/>
     <sheet name="profile1" sheetId="11" r:id="rId4"/>
     <sheet name="studyDesignII" sheetId="6" r:id="rId5"/>
-    <sheet name="studyDesignPopulations" sheetId="7" r:id="rId6"/>
-    <sheet name="studyDesignOE" sheetId="8" r:id="rId7"/>
-    <sheet name="studyDesignEstimands" sheetId="9" r:id="rId8"/>
-    <sheet name="studyDesignProcedures" sheetId="13" r:id="rId9"/>
-    <sheet name="studyDesignEncounters" sheetId="14" r:id="rId10"/>
-    <sheet name="studyDesignElements" sheetId="15" r:id="rId11"/>
-    <sheet name="configuration" sheetId="10" r:id="rId12"/>
+    <sheet name="studyDesignArms" sheetId="16" r:id="rId6"/>
+    <sheet name="studyDesignEpochs" sheetId="17" r:id="rId7"/>
+    <sheet name="studyDesignPopulations" sheetId="7" r:id="rId8"/>
+    <sheet name="studyDesignOE" sheetId="8" r:id="rId9"/>
+    <sheet name="studyDesignEstimands" sheetId="9" r:id="rId10"/>
+    <sheet name="studyDesignProcedures" sheetId="13" r:id="rId11"/>
+    <sheet name="studyDesignEncounters" sheetId="14" r:id="rId12"/>
+    <sheet name="studyDesignElements" sheetId="15" r:id="rId13"/>
+    <sheet name="configuration" sheetId="10" r:id="rId14"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -47,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="411" uniqueCount="244">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="441" uniqueCount="265">
   <si>
     <t>Epoch</t>
   </si>
@@ -779,6 +781,69 @@
   </si>
   <si>
     <t>The main design for the study</t>
+  </si>
+  <si>
+    <t>Data Generated Within Study</t>
+  </si>
+  <si>
+    <t>Data collected from subjects</t>
+  </si>
+  <si>
+    <t>Placebo Comparator Arm</t>
+  </si>
+  <si>
+    <t>Active Comparator Arm</t>
+  </si>
+  <si>
+    <t>Active Substance</t>
+  </si>
+  <si>
+    <t>studyArmDataOriginType</t>
+  </si>
+  <si>
+    <t>studyArmDataOriginDescription</t>
+  </si>
+  <si>
+    <t>studyArmType</t>
+  </si>
+  <si>
+    <t>studyArmDescription</t>
+  </si>
+  <si>
+    <t>studyArmName</t>
+  </si>
+  <si>
+    <t>FOLLOW-UP</t>
+  </si>
+  <si>
+    <t>Follow-up Epoch</t>
+  </si>
+  <si>
+    <t>TREATMENT</t>
+  </si>
+  <si>
+    <t>Treatment Epoch</t>
+  </si>
+  <si>
+    <t>BASELINE</t>
+  </si>
+  <si>
+    <t>Baseline Epoch</t>
+  </si>
+  <si>
+    <t>SCREENING</t>
+  </si>
+  <si>
+    <t>Screening Epoch</t>
+  </si>
+  <si>
+    <t>studyEpochType</t>
+  </si>
+  <si>
+    <t>studyEpochDescription</t>
+  </si>
+  <si>
+    <t>studyEpochName</t>
   </si>
 </sst>
 </file>
@@ -909,10 +974,10 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -1518,6 +1583,188 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DBFC82B4-C495-A142-993D-B6A47D77A4C3}">
+  <dimension ref="A1:H5"/>
+  <sheetViews>
+    <sheetView zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="6.83203125" customWidth="1"/>
+    <col min="2" max="2" width="22.5" customWidth="1"/>
+    <col min="3" max="4" width="23" customWidth="1"/>
+    <col min="5" max="5" width="28.1640625" customWidth="1"/>
+    <col min="6" max="7" width="17" customWidth="1"/>
+    <col min="8" max="8" width="61.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1" s="12" t="s">
+        <v>93</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>114</v>
+      </c>
+      <c r="C1" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="D1" s="13" t="s">
+        <v>115</v>
+      </c>
+      <c r="E1" s="13" t="s">
+        <v>123</v>
+      </c>
+      <c r="F1" s="13" t="s">
+        <v>117</v>
+      </c>
+      <c r="G1" s="13" t="s">
+        <v>99</v>
+      </c>
+      <c r="H1" s="13" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>118</v>
+      </c>
+      <c r="B2" t="s">
+        <v>122</v>
+      </c>
+      <c r="C2" t="s">
+        <v>119</v>
+      </c>
+      <c r="D2" t="s">
+        <v>120</v>
+      </c>
+      <c r="E2" t="s">
+        <v>124</v>
+      </c>
+      <c r="F2" t="s">
+        <v>95</v>
+      </c>
+      <c r="G2" t="s">
+        <v>102</v>
+      </c>
+      <c r="H2" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H3" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H4" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>153</v>
+      </c>
+      <c r="B5" t="s">
+        <v>154</v>
+      </c>
+      <c r="C5" t="s">
+        <v>119</v>
+      </c>
+      <c r="D5" t="s">
+        <v>155</v>
+      </c>
+      <c r="E5" t="s">
+        <v>156</v>
+      </c>
+      <c r="F5" t="s">
+        <v>97</v>
+      </c>
+      <c r="G5" t="s">
+        <v>103</v>
+      </c>
+      <c r="H5" t="s">
+        <v>157</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67C4BD8C-CCB1-D540-B5F1-57CAC0E84392}">
+  <dimension ref="A1:E5"/>
+  <sheetViews>
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="F25" sqref="F25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="7.33203125" customWidth="1"/>
+    <col min="2" max="2" width="17.5" customWidth="1"/>
+    <col min="3" max="3" width="27.33203125" customWidth="1"/>
+    <col min="4" max="4" width="24" style="7" customWidth="1"/>
+    <col min="5" max="5" width="29.6640625" customWidth="1"/>
+    <col min="6" max="6" width="14.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="B1" s="20" t="s">
+        <v>193</v>
+      </c>
+      <c r="C1" s="20" t="s">
+        <v>192</v>
+      </c>
+      <c r="D1" s="21" t="s">
+        <v>191</v>
+      </c>
+      <c r="E1" s="20" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>189</v>
+      </c>
+      <c r="B2" t="s">
+        <v>186</v>
+      </c>
+      <c r="C2" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>187</v>
+      </c>
+      <c r="B3" t="s">
+        <v>186</v>
+      </c>
+      <c r="C3" t="s">
+        <v>185</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>184</v>
+      </c>
+      <c r="E3" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B5" s="4"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{029D84EC-0EDA-504A-83E2-F11409AF2A05}">
   <dimension ref="A1:H6"/>
   <sheetViews>
@@ -1675,7 +1922,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FDB5F767-484F-2142-8F53-972CA3AC92C1}">
   <dimension ref="A1:E5"/>
   <sheetViews>
@@ -1781,7 +2028,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1886B59F-3C17-014D-9C61-BEC33F421A82}">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -1819,7 +2066,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{679CED36-1B68-6F40-B862-B156999A55CA}">
   <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <selection activeCell="B7" sqref="B7:E7"/>
     </sheetView>
   </sheetViews>
@@ -1856,34 +2103,34 @@
       <c r="A3" s="19" t="s">
         <v>35</v>
       </c>
-      <c r="B3" s="26" t="s">
+      <c r="B3" s="25" t="s">
         <v>158</v>
       </c>
-      <c r="C3" s="26"/>
-      <c r="D3" s="26"/>
-      <c r="E3" s="26"/>
+      <c r="C3" s="25"/>
+      <c r="D3" s="25"/>
+      <c r="E3" s="25"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="B4" s="25" t="s">
+      <c r="B4" s="26" t="s">
         <v>194</v>
       </c>
-      <c r="C4" s="25"/>
-      <c r="D4" s="25"/>
-      <c r="E4" s="25"/>
+      <c r="C4" s="26"/>
+      <c r="D4" s="26"/>
+      <c r="E4" s="26"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="B5" s="25" t="s">
+      <c r="B5" s="26" t="s">
         <v>144</v>
       </c>
-      <c r="C5" s="25"/>
-      <c r="D5" s="25"/>
-      <c r="E5" s="25"/>
+      <c r="C5" s="26"/>
+      <c r="D5" s="26"/>
+      <c r="E5" s="26"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="19" t="s">
@@ -2005,16 +2252,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="B9:E9"/>
+    <mergeCell ref="B10:E10"/>
+    <mergeCell ref="B8:E8"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="B5:E5"/>
     <mergeCell ref="B1:E1"/>
     <mergeCell ref="B2:E2"/>
     <mergeCell ref="B3:E3"/>
     <mergeCell ref="B6:E6"/>
     <mergeCell ref="B7:E7"/>
-    <mergeCell ref="B9:E9"/>
-    <mergeCell ref="B10:E10"/>
-    <mergeCell ref="B8:E8"/>
-    <mergeCell ref="B4:E4"/>
-    <mergeCell ref="B5:E5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2678,6 +2925,157 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FAA50C53-9694-7746-B056-40E562A4C352}">
+  <dimension ref="A1:E4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J30" sqref="J30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="17.83203125" style="3" customWidth="1"/>
+    <col min="2" max="2" width="24.83203125" style="3" customWidth="1"/>
+    <col min="3" max="3" width="23.5" style="3" customWidth="1"/>
+    <col min="4" max="4" width="32.1640625" style="3" customWidth="1"/>
+    <col min="5" max="5" width="25.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" s="23" t="s">
+        <v>253</v>
+      </c>
+      <c r="B1" s="23" t="s">
+        <v>252</v>
+      </c>
+      <c r="C1" s="23" t="s">
+        <v>251</v>
+      </c>
+      <c r="D1" s="23" t="s">
+        <v>250</v>
+      </c>
+      <c r="E1" s="23" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>248</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>247</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>245</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>245</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E4" s="11"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EAB445C9-60A6-D94F-B956-3A80A5E333DC}">
+  <dimension ref="A1:C5"/>
+  <sheetViews>
+    <sheetView topLeftCell="S1" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="18.33203125" customWidth="1"/>
+    <col min="2" max="2" width="27.6640625" customWidth="1"/>
+    <col min="3" max="3" width="18.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="23" t="s">
+        <v>264</v>
+      </c>
+      <c r="B1" s="23" t="s">
+        <v>263</v>
+      </c>
+      <c r="C1" s="23" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>261</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>259</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>257</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>255</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>254</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C037A932-CB5B-8D43-956E-5F5C367E07FC}">
   <dimension ref="A1:G4"/>
   <sheetViews>
@@ -2769,7 +3167,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B908C5D6-C6A1-4043-A49A-69C599CFBAE9}">
   <dimension ref="A1:G36"/>
   <sheetViews>
@@ -3177,186 +3575,4 @@
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DBFC82B4-C495-A142-993D-B6A47D77A4C3}">
-  <dimension ref="A1:H5"/>
-  <sheetViews>
-    <sheetView zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="6.83203125" customWidth="1"/>
-    <col min="2" max="2" width="22.5" customWidth="1"/>
-    <col min="3" max="4" width="23" customWidth="1"/>
-    <col min="5" max="5" width="28.1640625" customWidth="1"/>
-    <col min="6" max="7" width="17" customWidth="1"/>
-    <col min="8" max="8" width="61.83203125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A1" s="12" t="s">
-        <v>93</v>
-      </c>
-      <c r="B1" s="13" t="s">
-        <v>114</v>
-      </c>
-      <c r="C1" s="13" t="s">
-        <v>55</v>
-      </c>
-      <c r="D1" s="13" t="s">
-        <v>115</v>
-      </c>
-      <c r="E1" s="13" t="s">
-        <v>123</v>
-      </c>
-      <c r="F1" s="13" t="s">
-        <v>117</v>
-      </c>
-      <c r="G1" s="13" t="s">
-        <v>99</v>
-      </c>
-      <c r="H1" s="13" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>118</v>
-      </c>
-      <c r="B2" t="s">
-        <v>122</v>
-      </c>
-      <c r="C2" t="s">
-        <v>119</v>
-      </c>
-      <c r="D2" t="s">
-        <v>120</v>
-      </c>
-      <c r="E2" t="s">
-        <v>124</v>
-      </c>
-      <c r="F2" t="s">
-        <v>95</v>
-      </c>
-      <c r="G2" t="s">
-        <v>102</v>
-      </c>
-      <c r="H2" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="H3" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="H4" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>153</v>
-      </c>
-      <c r="B5" t="s">
-        <v>154</v>
-      </c>
-      <c r="C5" t="s">
-        <v>119</v>
-      </c>
-      <c r="D5" t="s">
-        <v>155</v>
-      </c>
-      <c r="E5" t="s">
-        <v>156</v>
-      </c>
-      <c r="F5" t="s">
-        <v>97</v>
-      </c>
-      <c r="G5" t="s">
-        <v>103</v>
-      </c>
-      <c r="H5" t="s">
-        <v>157</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67C4BD8C-CCB1-D540-B5F1-57CAC0E84392}">
-  <dimension ref="A1:E5"/>
-  <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="7.33203125" customWidth="1"/>
-    <col min="2" max="2" width="17.5" customWidth="1"/>
-    <col min="3" max="3" width="27.33203125" customWidth="1"/>
-    <col min="4" max="4" width="24" style="7" customWidth="1"/>
-    <col min="5" max="5" width="29.6640625" customWidth="1"/>
-    <col min="6" max="6" width="14.83203125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="B1" s="20" t="s">
-        <v>193</v>
-      </c>
-      <c r="C1" s="20" t="s">
-        <v>192</v>
-      </c>
-      <c r="D1" s="21" t="s">
-        <v>191</v>
-      </c>
-      <c r="E1" s="20" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>189</v>
-      </c>
-      <c r="B2" t="s">
-        <v>186</v>
-      </c>
-      <c r="C2" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>187</v>
-      </c>
-      <c r="B3" t="s">
-        <v>186</v>
-      </c>
-      <c r="C3" t="s">
-        <v>185</v>
-      </c>
-      <c r="D3" s="7" t="s">
-        <v>184</v>
-      </c>
-      <c r="E3" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B5" s="4"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>